<commit_message>
rest of the data
</commit_message>
<xml_diff>
--- a/Documentation/others/performance/values.xlsx
+++ b/Documentation/others/performance/values.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="9" uniqueCount="7">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="12" uniqueCount="7">
   <si>
     <t>CRANK-NICOLSON</t>
   </si>
@@ -978,7 +978,7 @@
         <v>1.541918900009126</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D15" si="1">A3</f>
+        <f t="shared" ref="D3:D14" si="1">A3</f>
         <v>2</v>
       </c>
       <c r="E3">
@@ -1029,7 +1029,7 @@
         <v>0.40253800000000001</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F3:F22" si="5">$E$2/E4</f>
+        <f t="shared" ref="F4:F22" si="5">$E$2/E4</f>
         <v>2.542145089407708</v>
       </c>
       <c r="G4">
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,12 +2299,579 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5.1887999999999997E-2</v>
+      </c>
+      <c r="C2">
+        <f>$B$2 /B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>9.7513199999999997E-4</v>
+      </c>
+      <c r="F2">
+        <f>$E$2/E2</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.341474</v>
+      </c>
+      <c r="I2">
+        <f>$H$2/H2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5.6606999999999998E-2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C15" si="0">$B$2 /B3</f>
+        <v>0.91663575176214951</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>7.6198599999999998E-4</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F22" si="1">$E$2/E3</f>
+        <v>1.2797242993965769</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.20078399999999999</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I16" si="2">$H$2/H3</f>
+        <v>1.7007032432863176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5.7411200000000003E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.90379577504041009</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>6.7186399999999999E-4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1.4513830179917364</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0.14574300000000001</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2.3429873132843428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5.9275899999999999E-2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.87536418679429573</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>6.8211599999999997E-4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>1.4295691641890822</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0.110064</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>3.1025039976740807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6.1346999999999999E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.84581153112621643</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6.7591699999999995E-4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1.4426800923782064</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>0.134552</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>2.5378589690231284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6.3687800000000003E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.81472432710817444</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6.9212899999999999E-4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>1.4088876495566578</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0.112706</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>3.0297765868720385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6.6121799999999994E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.78473362794116319</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>5.9008599999999997E-4</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.6525252251366751</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>0.103019</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>3.3146701093972957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6.7439100000000002E-2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.7694052856577267</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>7.7295300000000005E-4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.2615670034271165</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>8.3124199999999995E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>4.1079974303512099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>6.9764900000000005E-2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.74375509747738466</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>6.8807600000000003E-4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1.4171864735872199</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>0.100978</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>3.3816672938659909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>7.2472999999999996E-2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.71596318629006661</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>2.7971300000000001E-3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.34861876280330195</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>9.5677899999999996E-2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>3.568995556967701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>8.8842900000000002E-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.5840421688170917</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>6.8688400000000002E-4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>1.4196458208372884</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>6.7648899999999998E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>5.0477391354478787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>0.105517</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0.49175014452647436</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>1.32799E-3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.73429167388308647</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>6.9264199999999998E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>4.9300215695842873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0.14252000000000001</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.36407521751333144</v>
+      </c>
+      <c r="D14">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>9.1004400000000004E-4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1.0715218165275524</v>
+      </c>
+      <c r="G14">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>6.2262100000000001E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>5.4844600487294839</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>64</v>
+      </c>
+      <c r="B15">
+        <v>0.29300199999999998</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0.17709094135876205</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>5.6219099999999999E-3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.17345208301093401</v>
+      </c>
+      <c r="G15">
+        <v>32</v>
+      </c>
+      <c r="H15">
+        <v>6.7455100000000004E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>5.0622414020585538</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>1.1351099999999999E-3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.85906387927161243</v>
+      </c>
+      <c r="G16">
+        <v>64</v>
+      </c>
+      <c r="H16">
+        <v>0.113817</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>3.0002020787755783</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <v>1.1510800000000001E-3</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.84714528964103264</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>52</v>
+      </c>
+      <c r="E18">
+        <v>4.2808100000000003E-3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.2277914693714507</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19">
+        <v>9.4103800000000005E-4</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>1.0362302053689649</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>62</v>
+      </c>
+      <c r="E20">
+        <v>1.3349099999999999E-3</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0.73048520124952243</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <v>1.0600099999999999E-3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0.91992717049839157</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>64</v>
+      </c>
+      <c r="E22">
+        <v>6.4619999999999997E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1.5090250696378831E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Checked compiled with -O2 speedup
</commit_message>
<xml_diff>
--- a/Documentation/others/performance/values.xlsx
+++ b/Documentation/others/performance/values.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="5565" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="5565" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
     <sheet name="-O2" sheetId="2" r:id="rId2"/>
-    <sheet name="serial-parallel" sheetId="3" r:id="rId3"/>
-    <sheet name="-O2 1000" sheetId="4" r:id="rId4"/>
+    <sheet name="Simulation 10k" sheetId="5" r:id="rId3"/>
+    <sheet name="serial-parallel" sheetId="3" r:id="rId4"/>
+    <sheet name="-O2 1000" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="12" uniqueCount="7">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="18" uniqueCount="11">
   <si>
     <t>CRANK-NICOLSON</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>EXTERNAL</t>
+  </si>
+  <si>
+    <t>C-N</t>
+  </si>
+  <si>
+    <t>IU</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>CN</t>
   </si>
 </sst>
 </file>
@@ -894,7 +907,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1646,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I22"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,6 +2226,1129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F40" sqref="D26:F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.4902500000000001</v>
+      </c>
+      <c r="C2">
+        <f>$B$2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>95.731999999999999</v>
+      </c>
+      <c r="F2">
+        <f>$E$2/E2</f>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1.00437</v>
+      </c>
+      <c r="I2">
+        <f>$H$2/H2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.0143800000000001</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C15" si="0">$B$2/B3</f>
+        <v>1.4691239969242296</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>50.815199999999997</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F16" si="1">$E$2/E3</f>
+        <v>1.8839244950329823</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0.57217600000000002</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I22" si="2">$H$2/H3</f>
+        <v>1.7553515002376889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.85379099999999997</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1.7454505845107293</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>38.326599999999999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>2.4977952649074013</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>0.420568</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>2.3881274847349299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.75431199999999998</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1.9756413791640597</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>31.003</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>3.0878302099796793</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>0.31595899999999999</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>3.1787985149971991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.70869000000000004</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2.1028235194513822</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>30.3413</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>3.1551713341221372</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>0.25644099999999997</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>3.9165734028489987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.67159500000000005</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2.2189712549974314</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>27.585999999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>3.4703110273327051</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0.21798799999999999</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>4.6074554562636481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.64301699999999995</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.3175903591973466</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>21.943999999999999</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4.3625592417061609</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>0.18773100000000001</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>5.3500487399523786</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.625085</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.3840757656958655</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>22.522300000000001</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>4.2505427953628176</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0.165634</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>6.0637912505886469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.61571200000000004</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.4203686138974065</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>24.411899999999999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>3.9215300734477858</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>0.14877799999999999</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>6.750796488728172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.60982800000000004</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.4437218363210609</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>20.509</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>4.6678043785655081</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>0.13516700000000001</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>7.4305858678523595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>0.59441999999999995</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.5070657111133547</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>16.165800000000001</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>5.9218844721572701</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>8.9122099999999996E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>11.269595308010022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>0.60855099999999995</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.4488498088081365</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>13.2685</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>7.2149828541281984</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13">
+        <v>7.8432100000000005E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>12.805598728071796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0.62422</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.3873794495530425</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>11.5298</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>8.3030061232631969</v>
+      </c>
+      <c r="G14">
+        <v>32</v>
+      </c>
+      <c r="H14">
+        <v>5.3118899999999997E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>18.907959313916518</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>64</v>
+      </c>
+      <c r="B15">
+        <v>0.76497000000000004</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.9481156123769559</v>
+      </c>
+      <c r="D15">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <v>9.2682900000000004</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>10.328981937336875</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15">
+        <v>4.6128000000000002E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>21.77354318418314</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>64</v>
+      </c>
+      <c r="E16">
+        <v>5.1406299999999998</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>18.622620184685534</v>
+      </c>
+      <c r="G16">
+        <v>44</v>
+      </c>
+      <c r="H16">
+        <v>4.2021999999999997E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>23.901051829993815</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>48</v>
+      </c>
+      <c r="H17">
+        <v>3.9539100000000001E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>25.401943898571286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>52</v>
+      </c>
+      <c r="H18">
+        <v>3.8993100000000003E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>25.757634042946059</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>60</v>
+      </c>
+      <c r="H19">
+        <v>3.4657100000000003E-2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>28.98020896151149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>62</v>
+      </c>
+      <c r="H20">
+        <v>2.7419099999999998E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>36.630305152247885</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>63</v>
+      </c>
+      <c r="H21">
+        <v>2.9173999999999999E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>34.426886954137245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>64</v>
+      </c>
+      <c r="H22">
+        <v>9.3190899999999993E-2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>10.777554460789627</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1.9567000000000001E-2</v>
+      </c>
+      <c r="C26">
+        <f>$B$26/B26</f>
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0.85539600000000005</v>
+      </c>
+      <c r="F26">
+        <f>$E$26/E26</f>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1.925818E-2</v>
+      </c>
+      <c r="I26">
+        <f>$H$26/H26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>1.2921999999999999E-2</v>
+      </c>
+      <c r="C27">
+        <f>$B$26/B27</f>
+        <v>1.5142392818449157</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>0.50342799999999999</v>
+      </c>
+      <c r="F27">
+        <f>$E$26/E27</f>
+        <v>1.6991426778009966</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>6.6268400000000002E-3</v>
+      </c>
+      <c r="I27">
+        <f>$H$26/H27</f>
+        <v>2.9060879695299717</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>1.1003000000000001E-2</v>
+      </c>
+      <c r="C28">
+        <f>$B$26/B28</f>
+        <v>1.778333181859493</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>0.35936299999999999</v>
+      </c>
+      <c r="F28">
+        <f>$E$26/E28</f>
+        <v>2.3803118295428303</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>4.58217E-3</v>
+      </c>
+      <c r="I28">
+        <f>$H$26/H28</f>
+        <v>4.2028514873957095</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>1.03838E-2</v>
+      </c>
+      <c r="C29">
+        <f>$B$26/B29</f>
+        <v>1.8843775881661819</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>0.29151899999999997</v>
+      </c>
+      <c r="F29">
+        <f>$E$26/E29</f>
+        <v>2.9342718656416911</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>3.6859499999999999E-3</v>
+      </c>
+      <c r="I29">
+        <f>$H$26/H29</f>
+        <v>5.2247534556898492</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>1.0338999999999999E-2</v>
+      </c>
+      <c r="C30">
+        <f>$B$26/B30</f>
+        <v>1.8925427991101655</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>0.27585300000000001</v>
+      </c>
+      <c r="F30">
+        <f>$E$26/E30</f>
+        <v>3.1009124424965471</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="I30" t="e">
+        <f>$H$26/H30</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>1.01628E-2</v>
+      </c>
+      <c r="C31">
+        <f>$B$26/B31</f>
+        <v>1.925355217066163</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>0.25836799999999999</v>
+      </c>
+      <c r="F31">
+        <f>$E$26/E31</f>
+        <v>3.3107660391379743</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>2.6779199999999999E-3</v>
+      </c>
+      <c r="I31">
+        <f>$H$26/H31</f>
+        <v>7.1914694987154215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>1.0348100000000001E-2</v>
+      </c>
+      <c r="C32">
+        <f>$B$26/B32</f>
+        <v>1.8908785187618984</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <v>0.21065600000000001</v>
+      </c>
+      <c r="F32">
+        <f>$E$26/E32</f>
+        <v>4.0606296521342857</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <v>2.3210000000000001E-3</v>
+      </c>
+      <c r="I32">
+        <f>$H$26/H32</f>
+        <v>8.2973632055148645</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>1.056E-2</v>
+      </c>
+      <c r="C33">
+        <f>$B$26/B33</f>
+        <v>1.8529356060606061</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>0.18659999999999999</v>
+      </c>
+      <c r="F33">
+        <f>$E$26/E33</f>
+        <v>4.5841157556270105</v>
+      </c>
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>2.2201500000000002E-3</v>
+      </c>
+      <c r="I33">
+        <f>$H$26/H33</f>
+        <v>8.6742697565479805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>1.047739E-2</v>
+      </c>
+      <c r="C34">
+        <f>$B$26/B34</f>
+        <v>1.8675452569771671</v>
+      </c>
+      <c r="D34">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>0.18346899999999999</v>
+      </c>
+      <c r="F34">
+        <f>$E$26/E34</f>
+        <v>4.6623462274280669</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>1.9497900000000001E-3</v>
+      </c>
+      <c r="I34">
+        <f>$H$26/H34</f>
+        <v>9.8770534262664178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>1.1152E-2</v>
+      </c>
+      <c r="C35">
+        <f>$B$26/B35</f>
+        <v>1.7545731707317074</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>0.16852800000000001</v>
+      </c>
+      <c r="F35">
+        <f>$E$26/E35</f>
+        <v>5.0756906864141271</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>1.9080600000000001E-3</v>
+      </c>
+      <c r="I35">
+        <f>$H$26/H35</f>
+        <v>10.093068352148254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>1.3447000000000001E-2</v>
+      </c>
+      <c r="C36">
+        <f>$B$26/B36</f>
+        <v>1.4551201011378003</v>
+      </c>
+      <c r="D36">
+        <v>16</v>
+      </c>
+      <c r="E36">
+        <v>0.111919</v>
+      </c>
+      <c r="F36">
+        <f>$E$26/E36</f>
+        <v>7.6429918065743978</v>
+      </c>
+      <c r="G36">
+        <v>16</v>
+      </c>
+      <c r="H36">
+        <v>1.4619800000000001E-3</v>
+      </c>
+      <c r="I36">
+        <f>$H$26/H36</f>
+        <v>13.172669940765262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>1.6650000000000002E-2</v>
+      </c>
+      <c r="C37">
+        <f>$B$26/B37</f>
+        <v>1.1751951951951951</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
+      </c>
+      <c r="E37">
+        <v>6.9155900000000006E-2</v>
+      </c>
+      <c r="F37">
+        <f>$E$26/E37</f>
+        <v>12.369096490682645</v>
+      </c>
+      <c r="G37">
+        <v>20</v>
+      </c>
+      <c r="H37">
+        <v>4.0440600000000004E-3</v>
+      </c>
+      <c r="I37">
+        <f>$H$26/H37</f>
+        <v>4.7620905723456124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>32</v>
+      </c>
+      <c r="B38">
+        <v>2.4313000000000001E-2</v>
+      </c>
+      <c r="C38">
+        <f>$B$26/B38</f>
+        <v>0.80479578826142395</v>
+      </c>
+      <c r="D38">
+        <v>24</v>
+      </c>
+      <c r="E38">
+        <v>6.2262100000000001E-2</v>
+      </c>
+      <c r="F38">
+        <f>$E$26/E38</f>
+        <v>13.738630723987788</v>
+      </c>
+      <c r="G38">
+        <v>32</v>
+      </c>
+      <c r="H38">
+        <v>1.93852E-3</v>
+      </c>
+      <c r="I38">
+        <f>$H$26/H38</f>
+        <v>9.9344757856509087</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>64</v>
+      </c>
+      <c r="B39">
+        <v>9.7736100000000006E-2</v>
+      </c>
+      <c r="C39">
+        <f>$B$26/B39</f>
+        <v>0.20020238171975349</v>
+      </c>
+      <c r="D39">
+        <v>32</v>
+      </c>
+      <c r="E39">
+        <v>0.10100099999999999</v>
+      </c>
+      <c r="F39">
+        <f>$E$26/E39</f>
+        <v>8.4691834734309577</v>
+      </c>
+      <c r="G39">
+        <v>40</v>
+      </c>
+      <c r="H39">
+        <v>4.1460999999999998E-3</v>
+      </c>
+      <c r="I39">
+        <f>$H$26/H39</f>
+        <v>4.6448903789103015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>64</v>
+      </c>
+      <c r="E40">
+        <v>0.13538</v>
+      </c>
+      <c r="F40">
+        <f>$E$26/E40</f>
+        <v>6.3184813118629046</v>
+      </c>
+      <c r="G40">
+        <v>44</v>
+      </c>
+      <c r="H40">
+        <v>1.8160299999999999E-3</v>
+      </c>
+      <c r="I40">
+        <f>$H$26/H40</f>
+        <v>10.604549484314687</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>48</v>
+      </c>
+      <c r="H41">
+        <v>1.7499900000000001E-3</v>
+      </c>
+      <c r="I41">
+        <f>$H$26/H41</f>
+        <v>11.004737169926685</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>52</v>
+      </c>
+      <c r="H42">
+        <v>3.3588400000000001E-3</v>
+      </c>
+      <c r="I42">
+        <f>$H$26/H42</f>
+        <v>5.7335806409355605</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>60</v>
+      </c>
+      <c r="H43">
+        <v>2.55704E-3</v>
+      </c>
+      <c r="I43">
+        <f>$H$26/H43</f>
+        <v>7.5314347839689644</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>62</v>
+      </c>
+      <c r="H44">
+        <v>1.54495E-3</v>
+      </c>
+      <c r="I44">
+        <f>$H$26/H44</f>
+        <v>12.465244829929771</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>63</v>
+      </c>
+      <c r="H45">
+        <v>1.6629699999999999E-3</v>
+      </c>
+      <c r="I45">
+        <f>$H$26/H45</f>
+        <v>11.580593756952922</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>64</v>
+      </c>
+      <c r="H46">
+        <v>6.0019000000000003E-2</v>
+      </c>
+      <c r="I46">
+        <f>$H$26/H46</f>
+        <v>0.32086805844815808</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2297,11 +3433,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A2:C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>